<commit_message>
excel y orden de reporte
</commit_message>
<xml_diff>
--- a/formatos/editar-user.xlsx
+++ b/formatos/editar-user.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Factoria - Digtl01\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\cursodelosi-github\formatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="23715" windowHeight="10050" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="23715" windowHeight="10050"/>
   </bookViews>
   <sheets>
     <sheet name="Lista" sheetId="1" r:id="rId1"/>
@@ -215,7 +215,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -256,6 +256,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -565,13 +571,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" style="17" customWidth="1"/>
     <col min="2" max="2" width="19" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
@@ -585,7 +591,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:42" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="16" t="s">
         <v>24</v>
       </c>
       <c r="B1" s="6" t="s">
@@ -661,7 +667,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K10803"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>

</xml_diff>